<commit_message>
Update_Student_details fundtion is added
</commit_message>
<xml_diff>
--- a/data/students.xlsx
+++ b/data/students.xlsx
@@ -525,10 +525,10 @@
         <v>28</v>
       </c>
       <c r="J2" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="K2" t="n">
-        <v>89</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>